<commit_message>
fixed add private segments for appnexus
</commit_message>
<xml_diff>
--- a/to_return/Test_AppNexus_Add_UploadTemplate_UPLOAD_Segment_output_add_segments.xlsx
+++ b/to_return/Test_AppNexus_Add_UploadTemplate_UPLOAD_Segment_output_add_segments.xlsx
@@ -58,10 +58,10 @@
     <t>Add Billing Response</t>
   </si>
   <si>
-    <t>Eyeota - US 33Across - B2B - Healthcare Dentist</t>
-  </si>
-  <si>
-    <t>Sub Healthcare Dentist</t>
+    <t>Eyeota - US 33Across - B2B - Healthcare Executives</t>
+  </si>
+  <si>
+    <t>Leadership + Healthcare Executives</t>
   </si>
   <si>
     <t>active</t>
@@ -483,10 +483,10 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2">
-        <v>15651519</v>
+        <v>15651527</v>
       </c>
       <c r="B2">
-        <v>-2147370270</v>
+        <v>-2147370268</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>

</xml_diff>